<commit_message>
Improved accuracy of ingredient measurements.
</commit_message>
<xml_diff>
--- a/Data/emissions.xlsx
+++ b/Data/emissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF2E603-45B7-46B7-A3FB-C2D135242186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4EEFC7-6974-4945-938C-A64A79F80B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{45F902C0-B639-4689-A03F-C4EBE431CFD7}"/>
   </bookViews>
@@ -530,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D879B48-85B0-4B2A-9B64-5F6B6417E8CC}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="325" zoomScaleNormal="325" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,6 +1080,12 @@
         <v>1.81</v>
       </c>
     </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <f>AVERAGE(D2:D45)+1.9</f>
+        <v>5.3367904544784208</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added file tree diagram.
</commit_message>
<xml_diff>
--- a/Data/emissions.xlsx
+++ b/Data/emissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AA5CA7-770A-44FF-AA3B-D292A7DA950D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9491A76-A8B2-4539-B59B-F4835B22EF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{45F902C0-B639-4689-A03F-C4EBE431CFD7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Food type</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>banana</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -541,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D879B48-85B0-4B2A-9B64-5F6B6417E8CC}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1113,7 +1116,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>51</v>
+      </c>
       <c r="D50">
         <f>AVERAGE(D2:D45)+1.9</f>
         <v>5.3367904544784208</v>

</xml_diff>